<commit_message>
Add Spark Practice labs
</commit_message>
<xml_diff>
--- a/Class-Room-Files/Hadoop Intro.xlsx
+++ b/Class-Room-Files/Hadoop Intro.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\github\Data-Engineering\Class-Room-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C0BE368-D8F6-4880-831D-939DE97381BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EEEE31-161A-4EFB-9E14-8CFCFF7A6020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED981B86-E7B9-43F4-9502-D992494B95BE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{ED981B86-E7B9-43F4-9502-D992494B95BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="316">
   <si>
     <t>Server
 Ram
@@ -903,12 +904,96 @@
   <si>
     <t>JOINS, SUB QUERIES, WINDOW FUNCTIONS (RANK, DENSE_RANK, ROW_NUMBER, LEAD AND LAG)</t>
   </si>
+  <si>
+    <t>400 MB</t>
+  </si>
+  <si>
+    <t>ADLS/HDFS</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>3 replication</t>
+  </si>
+  <si>
+    <t>4 bloks * 3</t>
+  </si>
+  <si>
+    <t>filtering</t>
+  </si>
+  <si>
+    <t>toLowercase</t>
+  </si>
+  <si>
+    <t>writeToDisk</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>baseDataset</t>
+  </si>
+  <si>
+    <t>P1 (100)</t>
+  </si>
+  <si>
+    <t>P1 (10)</t>
+  </si>
+  <si>
+    <t>P1(10)</t>
+  </si>
+  <si>
+    <t>P2 (1000)</t>
+  </si>
+  <si>
+    <t>P3 (500)</t>
+  </si>
+  <si>
+    <t>P4 (30)</t>
+  </si>
+  <si>
+    <t>P3 (20)</t>
+  </si>
+  <si>
+    <t>P4 (0)</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>P4 (20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val myDS= </t>
+  </si>
+  <si>
+    <t xml:space="preserve">val myFilteredDS = </t>
+  </si>
+  <si>
+    <t>myFilteredDS.methods</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,8 +1021,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,8 +1054,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1028,11 +1138,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1062,6 +1202,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1786,6 +1937,473 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604157</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>103415</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34999476-59BB-425F-B8D1-D0B1649BE165}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4441371" y="3532414"/>
+          <a:ext cx="4528458" cy="348343"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593446</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>116403</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>92704</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>64943</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E7FBD65-0ECC-498E-ADC0-05F69757C40F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4438082" y="3961039"/>
+          <a:ext cx="4534520" cy="312222"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>602625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>116403</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>109503</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>59228</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE2769B-5B61-408D-B359-4B3C39F2F007}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4447261" y="4324721"/>
+          <a:ext cx="4542140" cy="306507"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>591688</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>79811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>87111</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>63211</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle: Rounded Corners 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0197DBA-3FDB-426E-AA93-64A10FC2C425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4436324" y="6305697"/>
+          <a:ext cx="5781923" cy="347082"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>589636</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>116403</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>77932</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>63038</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle: Rounded Corners 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F7DE2DC-D4B4-4A67-9F7A-93D740E43B08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4434272" y="6705971"/>
+          <a:ext cx="5774796" cy="310317"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600720</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>116403</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>186171</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>55418</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle: Rounded Corners 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E6AD405-17A6-424F-A6DD-18EC503585D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4445356" y="7069653"/>
+          <a:ext cx="5871951" cy="302697"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>574889</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>75482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76027</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>55072</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle: Rounded Corners 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B367701B-600E-4375-97DB-2C379726D722}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419525" y="6301368"/>
+          <a:ext cx="5787638" cy="343272"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2085,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889A36E0-8E36-4B3B-9543-C5D57EC06C45}">
   <dimension ref="A5:Q509"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3844,4 +4462,549 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E596C3-26BA-433F-BA59-BBE6BAE14451}">
+  <dimension ref="B2:P52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5">
+        <f>400/100</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="M10" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>298</v>
+      </c>
+      <c r="J19" t="s">
+        <v>299</v>
+      </c>
+      <c r="L19" t="s">
+        <v>300</v>
+      </c>
+      <c r="N19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" t="s">
+        <v>296</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H22" s="18"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>293</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="M23" s="23"/>
+      <c r="N23" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>302</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>294</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I25" s="23"/>
+      <c r="J25" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="M25" s="23"/>
+      <c r="N25" s="26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H26" s="18"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>295</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="N27" s="19"/>
+    </row>
+    <row r="34" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>298</v>
+      </c>
+      <c r="J34" t="s">
+        <v>299</v>
+      </c>
+      <c r="L34" t="s">
+        <v>300</v>
+      </c>
+      <c r="N34" t="s">
+        <v>301</v>
+      </c>
+      <c r="P34" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="P35" s="17"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" t="s">
+        <v>296</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="I36" s="23"/>
+      <c r="J36" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="K36" s="23"/>
+      <c r="L36" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="M36" s="23"/>
+      <c r="P36" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H37" s="18"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="23"/>
+      <c r="P37" s="18"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>314</v>
+      </c>
+      <c r="F38" t="s">
+        <v>293</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="I38" s="23"/>
+      <c r="J38" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="M38" s="23"/>
+      <c r="P38" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H39" s="18"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="23"/>
+      <c r="P39" s="18"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>315</v>
+      </c>
+      <c r="F40" t="s">
+        <v>294</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I40" s="23"/>
+      <c r="J40" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="K40" s="23"/>
+      <c r="L40" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="M40" s="23"/>
+      <c r="P40" s="26" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H41" s="18"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="23"/>
+      <c r="P41" s="18"/>
+    </row>
+    <row r="42" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>295</v>
+      </c>
+      <c r="H42" s="27"/>
+      <c r="J42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="P42" s="19"/>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" t="s">
+        <v>36</v>
+      </c>
+      <c r="L45" t="s">
+        <v>37</v>
+      </c>
+      <c r="N45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H46" s="20"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K46" s="21"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="20"/>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H47" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I47" s="21"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M47" s="21"/>
+      <c r="N47" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H48" s="20"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" s="21"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="20"/>
+    </row>
+    <row r="49" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H49" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49" s="21"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="20"/>
+    </row>
+    <row r="50" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="21"/>
+      <c r="J50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="L50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" s="21"/>
+      <c r="N50" s="20"/>
+    </row>
+    <row r="51" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H51" s="22"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="M51" s="21"/>
+      <c r="N51" s="22"/>
+    </row>
+    <row r="52" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H52" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="I52" s="21"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>